<commit_message>
Also test SuperLinq's UpdatablePriorityQueue
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\github\danielearwicker\PriorityQueueMergeSort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68409CA-24C4-490A-8AB3-EDB921973A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A754EC53-1EB8-4852-979B-355565C59874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CF49712B-A321-44A5-9207-24724962BC33}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CF49712B-A321-44A5-9207-24724962BC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Chunks</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>IEnumerable</t>
+  </si>
+  <si>
+    <t>UpdatablePriorityQueue</t>
   </si>
 </sst>
 </file>
@@ -235,10 +238,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$17</c:f>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -280,45 +283,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$17</c:f>
+              <c:f>Sheet1!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>18.723972</c:v>
+                  <c:v>18.529098000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.599968000000001</c:v>
+                  <c:v>27.356054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.801421999999999</c:v>
+                  <c:v>30.419274000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.126619999999903</c:v>
+                  <c:v>35.552033999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.484843999999903</c:v>
+                  <c:v>47.091551999999901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.036829999999902</c:v>
+                  <c:v>49.689511999999901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.738320000000002</c:v>
+                  <c:v>53.343269999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.230781999999905</c:v>
+                  <c:v>61.162908000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>68.799373999999901</c:v>
+                  <c:v>64.723568</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>101.856563999999</c:v>
+                  <c:v>102.317274</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>125.400902</c:v>
+                  <c:v>126.876662</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>176.83000399999901</c:v>
+                  <c:v>180.19378599999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,10 +365,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$17</c:f>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -407,45 +410,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$17</c:f>
+              <c:f>Sheet1!$C$4:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>22.301964000000002</c:v>
+                  <c:v>22.220531999999899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.011686000000001</c:v>
+                  <c:v>26.285028000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.106043999999901</c:v>
+                  <c:v>28.258835999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.182501999999999</c:v>
+                  <c:v>29.412277999999901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.058233999999999</c:v>
+                  <c:v>34.779199999999904</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.464112</c:v>
+                  <c:v>34.9364419999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.260173999999999</c:v>
+                  <c:v>35.555840000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.753383999999997</c:v>
+                  <c:v>37.306153999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.002147999999998</c:v>
+                  <c:v>37.524374000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.227029999999999</c:v>
+                  <c:v>44.311413999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47.379673999999902</c:v>
+                  <c:v>47.622579999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.19415</c:v>
+                  <c:v>50.111398000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,6 +457,133 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3C98-4CC3-9214-02FAF38787D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>UpdatablePriorityQueue</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>85.66104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.584378000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.896268000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100.815382</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>127.01478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.945911999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122.200549999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125.552784</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130.64650999999901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>144.31034600000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>142.786644</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>165.05588599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-899E-4D9B-948C-60D9BBA2685F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -782,10 +912,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -827,45 +957,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$B$32</c:f>
+              <c:f>Sheet1!$B$19:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>10.343102</c:v>
+                  <c:v>10.952731999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.305883999999999</c:v>
+                  <c:v>20.815279999999898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.571586</c:v>
+                  <c:v>22.280327999999901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.777757999999999</c:v>
+                  <c:v>29.836098</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.6465859999999</c:v>
+                  <c:v>38.416268000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.816233999999902</c:v>
+                  <c:v>42.862541999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.144713999999901</c:v>
+                  <c:v>42.060617999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46.8398579999999</c:v>
+                  <c:v>49.335949999999897</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.992607999999898</c:v>
+                  <c:v>52.049443999999902</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>77.780929999999998</c:v>
+                  <c:v>78.651239999999902</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>97.387225999999998</c:v>
+                  <c:v>98.492193999999898</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>144.50746599999999</c:v>
+                  <c:v>148.73483399999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,10 +1039,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$19:$A$32</c:f>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -954,45 +1084,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$32</c:f>
+              <c:f>Sheet1!$C$19:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>11.989541999999901</c:v>
+                  <c:v>12.100931999999901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.67727</c:v>
+                  <c:v>20.704621999999901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.990735999999998</c:v>
+                  <c:v>21.948605999999899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.981705999999999</c:v>
+                  <c:v>28.945848000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>35.558886000000001</c:v>
+                  <c:v>39.283358</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.088419999999999</c:v>
+                  <c:v>43.680300000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.630122</c:v>
+                  <c:v>41.717243999999901</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.373371999999897</c:v>
+                  <c:v>43.007722000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.440663999999998</c:v>
+                  <c:v>42.203471999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47.803815999999998</c:v>
+                  <c:v>48.445879999999903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.387507999999997</c:v>
+                  <c:v>50.701616000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>61.442568000000001</c:v>
+                  <c:v>60.254711999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,6 +1131,133 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9869-420C-B5ED-A81EAA400ACA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>UpdatablePriorityQueue</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$19:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19.415455999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.746286000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.6240179999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.460520000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.757621999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.510322000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51.119397999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54.436589999999903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>54.687125999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.892561999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.751185999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>77.804056000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-37E6-47F4-8B74-652CC31A2AD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4548,16 +4805,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482738</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>204580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>511314</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4584,16 +4841,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480252</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>201268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>158749</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>534227</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>55218</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4620,16 +4877,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>477768</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>199335</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>196849</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>588893</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>154885</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4656,16 +4913,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469761</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>304523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>196849</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>599936</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>84205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4990,10 +5247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA224BD-B6BA-4692-B735-73E3E79DC4FC}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5002,7 +5259,7 @@
     <col min="3" max="3" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5012,284 +5269,359 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>18.723972</v>
+        <v>18.529098000000001</v>
       </c>
       <c r="C4">
-        <v>22.301964000000002</v>
+        <v>22.220531999999899</v>
+      </c>
+      <c r="D4">
+        <v>85.66104</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>28.599968000000001</v>
+        <v>27.356054</v>
       </c>
       <c r="C5">
-        <v>26.011686000000001</v>
+        <v>26.285028000000001</v>
+      </c>
+      <c r="D5">
+        <v>92.584378000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>31.801421999999999</v>
+        <v>30.419274000000001</v>
       </c>
       <c r="C6">
-        <v>27.106043999999901</v>
+        <v>28.258835999999999</v>
+      </c>
+      <c r="D6">
+        <v>94.896268000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>37.126619999999903</v>
+        <v>35.552033999999999</v>
       </c>
       <c r="C7">
-        <v>29.182501999999999</v>
+        <v>29.412277999999901</v>
+      </c>
+      <c r="D7">
+        <v>100.815382</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>47.484843999999903</v>
+        <v>47.091551999999901</v>
       </c>
       <c r="C8">
-        <v>34.058233999999999</v>
+        <v>34.779199999999904</v>
+      </c>
+      <c r="D8">
+        <v>127.01478</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>52.036829999999902</v>
+        <v>49.689511999999901</v>
       </c>
       <c r="C9">
-        <v>35.464112</v>
+        <v>34.9364419999999</v>
+      </c>
+      <c r="D9">
+        <v>119.945911999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>56.738320000000002</v>
+        <v>53.343269999999997</v>
       </c>
       <c r="C10">
-        <v>36.260173999999999</v>
+        <v>35.555840000000003</v>
+      </c>
+      <c r="D10">
+        <v>122.200549999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>64.230781999999905</v>
+        <v>61.162908000000002</v>
       </c>
       <c r="C11">
-        <v>36.753383999999997</v>
+        <v>37.306153999999999</v>
+      </c>
+      <c r="D11">
+        <v>125.552784</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>68.799373999999901</v>
+        <v>64.723568</v>
       </c>
       <c r="C12">
-        <v>38.002147999999998</v>
+        <v>37.524374000000002</v>
+      </c>
+      <c r="D12">
+        <v>130.64650999999901</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>101.856563999999</v>
+        <v>102.317274</v>
       </c>
       <c r="C13">
-        <v>44.227029999999999</v>
+        <v>44.311413999999999</v>
+      </c>
+      <c r="D13">
+        <v>144.31034600000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14">
-        <v>125.400902</v>
+        <v>126.876662</v>
       </c>
       <c r="C14">
-        <v>47.379673999999902</v>
+        <v>47.622579999999999</v>
+      </c>
+      <c r="D14">
+        <v>142.786644</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>30</v>
       </c>
       <c r="B15">
-        <v>176.83000399999901</v>
+        <v>180.19378599999999</v>
       </c>
       <c r="C15">
-        <v>50.19415</v>
+        <v>50.111398000000001</v>
+      </c>
+      <c r="D15">
+        <v>165.05588599999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19">
-        <v>10.343102</v>
+        <v>10.952731999999999</v>
       </c>
       <c r="C19">
-        <v>11.989541999999901</v>
+        <v>12.100931999999901</v>
+      </c>
+      <c r="D19">
+        <v>19.415455999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20">
-        <v>18.305883999999999</v>
+        <v>20.815279999999898</v>
       </c>
       <c r="C20">
-        <v>19.67727</v>
+        <v>20.704621999999901</v>
+      </c>
+      <c r="D20">
+        <v>30.746286000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21">
-        <v>20.571586</v>
+        <v>22.280327999999901</v>
       </c>
       <c r="C21">
-        <v>20.990735999999998</v>
+        <v>21.948605999999899</v>
+      </c>
+      <c r="D21">
+        <v>31.6240179999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22">
-        <v>25.777757999999999</v>
+        <v>29.836098</v>
       </c>
       <c r="C22">
-        <v>25.981705999999999</v>
+        <v>28.945848000000002</v>
+      </c>
+      <c r="D22">
+        <v>40.460520000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
       <c r="B23">
-        <v>33.6465859999999</v>
+        <v>38.416268000000002</v>
       </c>
       <c r="C23">
-        <v>35.558886000000001</v>
+        <v>39.283358</v>
+      </c>
+      <c r="D23">
+        <v>50.757621999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
       <c r="B24">
-        <v>38.816233999999902</v>
+        <v>42.862541999999998</v>
       </c>
       <c r="C24">
-        <v>39.088419999999999</v>
+        <v>43.680300000000003</v>
+      </c>
+      <c r="D24">
+        <v>52.510322000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25">
-        <v>40.144713999999901</v>
+        <v>42.060617999999998</v>
       </c>
       <c r="C25">
-        <v>38.630122</v>
+        <v>41.717243999999901</v>
+      </c>
+      <c r="D25">
+        <v>51.119397999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26">
-        <v>46.8398579999999</v>
+        <v>49.335949999999897</v>
       </c>
       <c r="C26">
-        <v>41.373371999999897</v>
+        <v>43.007722000000001</v>
+      </c>
+      <c r="D26">
+        <v>54.436589999999903</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27">
-        <v>49.992607999999898</v>
+        <v>52.049443999999902</v>
       </c>
       <c r="C27">
-        <v>40.440663999999998</v>
+        <v>42.203471999999998</v>
+      </c>
+      <c r="D27">
+        <v>54.687125999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>15</v>
       </c>
       <c r="B28">
-        <v>77.780929999999998</v>
+        <v>78.651239999999902</v>
       </c>
       <c r="C28">
-        <v>47.803815999999998</v>
+        <v>48.445879999999903</v>
+      </c>
+      <c r="D28">
+        <v>60.892561999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>20</v>
       </c>
       <c r="B29">
-        <v>97.387225999999998</v>
+        <v>98.492193999999898</v>
       </c>
       <c r="C29">
-        <v>49.387507999999997</v>
+        <v>50.701616000000001</v>
+      </c>
+      <c r="D29">
+        <v>62.751185999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30">
-        <v>144.50746599999999</v>
+        <v>148.73483399999901</v>
       </c>
       <c r="C30">
-        <v>61.442568000000001</v>
+        <v>60.254711999999998</v>
+      </c>
+      <c r="D30">
+        <v>77.804056000000003</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>